<commit_message>
split the UPDATE SQL file into separate files for each table. updated charts to imprint the date stamp, delete SVG & retain PDF. tidied README to be more concise compared to new DOCX file, charts.
</commit_message>
<xml_diff>
--- a/playstation/output/wishlist.xlsx
+++ b/playstation/output/wishlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2024-12-04" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2024-12-11" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="wishlist" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="5"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>

</xml_diff>

<commit_message>
first update of 2025 (January) - reconciled pricing values between Excel & SQL (updated values were not entered into SQL previously) - ranking system TBC in next commit (along with other small updates)
</commit_message>
<xml_diff>
--- a/playstation/output/wishlist.xlsx
+++ b/playstation/output/wishlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2024-12-31" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2025-01-31" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="wishlist" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -107,72 +107,63 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>Disney Epic Mickey: Rebrushed</t>
+    <t>Gex Trilogy</t>
+  </si>
+  <si>
+    <t>Crystal Dynamics</t>
+  </si>
+  <si>
+    <t>Ghost of Yotei</t>
+  </si>
+  <si>
+    <t>Sucker Punch Productions</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto VI</t>
+  </si>
+  <si>
+    <t>Rockstar North</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Haunted Chocolatier</t>
+  </si>
+  <si>
+    <t>TBR 2026</t>
+  </si>
+  <si>
+    <t>ConcernedApe (Eric Barone)</t>
+  </si>
+  <si>
+    <t>Intergalactic</t>
+  </si>
+  <si>
+    <t>Naughty Dog</t>
+  </si>
+  <si>
+    <t>Legacy of Kain: Soul Reaver</t>
+  </si>
+  <si>
+    <t>Legacy of Kain: Soul Reaver 2</t>
+  </si>
+  <si>
+    <t>PS2</t>
+  </si>
+  <si>
+    <t>Life is Strange: Double Exposure</t>
+  </si>
+  <si>
+    <t>Deck Nine</t>
+  </si>
+  <si>
+    <t>Looney Tunes: Wacky World of Sports</t>
   </si>
   <si>
     <t>PS4</t>
   </si>
   <si>
-    <t>Purple Lamp Studios</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Gex Trilogy</t>
-  </si>
-  <si>
-    <t>Crystal Dynamics</t>
-  </si>
-  <si>
-    <t>Ghost of Yotei</t>
-  </si>
-  <si>
-    <t>Sucker Punch Productions</t>
-  </si>
-  <si>
-    <t>Grand Theft Auto VI</t>
-  </si>
-  <si>
-    <t>Rockstar North</t>
-  </si>
-  <si>
-    <t>Scotland</t>
-  </si>
-  <si>
-    <t>Haunted Chocolatier</t>
-  </si>
-  <si>
-    <t>TBR 2026</t>
-  </si>
-  <si>
-    <t>ConcernedApe (Eric Barone)</t>
-  </si>
-  <si>
-    <t>Intergalactic</t>
-  </si>
-  <si>
-    <t>Naughty Dog</t>
-  </si>
-  <si>
-    <t>Legacy of Kain: Soul Reaver</t>
-  </si>
-  <si>
-    <t>Legacy of Kain: Soul Reaver 2</t>
-  </si>
-  <si>
-    <t>PS2</t>
-  </si>
-  <si>
-    <t>Life is Strange: Double Exposure</t>
-  </si>
-  <si>
-    <t>Deck Nine</t>
-  </si>
-  <si>
-    <t>Looney Tunes: Wacky World of Sports</t>
-  </si>
-  <si>
     <t>Bamtang Games</t>
   </si>
   <si>
@@ -185,6 +176,12 @@
     <t>Insomniac Games</t>
   </si>
   <si>
+    <t>Medievil 2</t>
+  </si>
+  <si>
+    <t>Guerrilla Cambridge (SCE Studio Cambridge)</t>
+  </si>
+  <si>
     <t>Monster Prom 2: Monster Camp: XXL</t>
   </si>
   <si>
@@ -227,15 +224,33 @@
     <t>Germany</t>
   </si>
   <si>
+    <t>The Wolf Among Us Season 2 TTG</t>
+  </si>
+  <si>
+    <t>Telltale Games</t>
+  </si>
+  <si>
+    <t>Two Point Museum</t>
+  </si>
+  <si>
+    <t>Two Point Studios</t>
+  </si>
+  <si>
+    <t>Witchbrook</t>
+  </si>
+  <si>
+    <t>Chucklefish</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>The Sims 4: For Rent Expansion</t>
   </si>
   <si>
     <t>DLC</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Maxis</t>
   </si>
   <si>
@@ -254,37 +269,25 @@
     <t>The Sims 4: Lovestruck Expansion</t>
   </si>
   <si>
-    <t>The Wolf Among Us Season 2 TTG</t>
-  </si>
-  <si>
-    <t>Telltale Games</t>
-  </si>
-  <si>
-    <t>Two Point Museum</t>
-  </si>
-  <si>
-    <t>Two Point Studios</t>
-  </si>
-  <si>
-    <t>TY The Tasmanian Tiger 2: Bush Rescue</t>
-  </si>
-  <si>
-    <t>Krome Studios</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Witchbrook</t>
-  </si>
-  <si>
-    <t>Chucklefish</t>
-  </si>
-  <si>
-    <t>Like a Dragon: Pirate Yakuza in Hawaii</t>
-  </si>
-  <si>
-    <t>Ryu Ga Gotoku Studio</t>
+    <t>Need for Speed Hot Pursuit</t>
+  </si>
+  <si>
+    <t>PS3</t>
+  </si>
+  <si>
+    <t>Criterion Games</t>
+  </si>
+  <si>
+    <t>High on Life</t>
+  </si>
+  <si>
+    <t>Squanch Games</t>
+  </si>
+  <si>
+    <t>Pac-Man World: Re-Pac</t>
+  </si>
+  <si>
+    <t>Now Production</t>
   </si>
   <si>
     <t>Legend of Zelda: Tears of the Kingdom</t>
@@ -363,7 +366,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,8 +381,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -390,14 +393,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -419,12 +428,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -473,68 +493,68 @@
     <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="4" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="10" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -791,7 +811,7 @@
     <col customWidth="1" min="10" max="10" width="7.88"/>
     <col customWidth="1" min="11" max="11" width="6.63"/>
     <col customWidth="1" min="12" max="12" width="6.88"/>
-    <col customWidth="1" min="13" max="13" width="24.13"/>
+    <col customWidth="1" min="13" max="13" width="38.13"/>
     <col customWidth="1" min="14" max="14" width="8.38"/>
   </cols>
   <sheetData>
@@ -841,7 +861,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1052.0</v>
+        <v>1057.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -865,18 +885,18 @@
         <v>59.99</v>
       </c>
       <c r="I2" s="6">
-        <v>29.99</v>
+        <v>59.99</v>
       </c>
       <c r="J2" s="7">
         <f t="shared" ref="J2:J32" si="1">H2-I2</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K2" s="8">
         <v>1.0</v>
       </c>
       <c r="L2" s="9">
-        <f t="shared" ref="L2:L32" si="2">I2/K2</f>
-        <v>29.99</v>
+        <f t="shared" ref="L2:L31" si="2">I2/K2</f>
+        <v>59.99</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>18</v>
@@ -887,7 +907,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1053.0</v>
+        <v>1058.0</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>20</v>
@@ -913,7 +933,7 @@
       <c r="I3" s="6">
         <v>79.99</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -932,8 +952,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12">
-        <v>1054.0</v>
+      <c r="A4" s="4">
+        <v>1059.0</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>24</v>
@@ -941,47 +961,47 @@
       <c r="C4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="11">
         <v>35699.0</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="6">
         <v>19.99</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="6">
         <v>19.99</v>
       </c>
-      <c r="J4" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="L4" s="16">
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L4" s="9">
         <f t="shared" si="2"/>
         <v>19.99</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>1055.0</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>1060.0</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1003,18 +1023,18 @@
         <v>79.99</v>
       </c>
       <c r="I5" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39.99</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="K5" s="8">
         <v>1.0</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="2"/>
-        <v>79.99</v>
+        <v>39.99</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>29</v>
@@ -1025,59 +1045,59 @@
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>1056.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>1061.0</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="6">
+        <v>19.99</v>
+      </c>
+      <c r="I6" s="6">
+        <v>19.99</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="2"/>
+        <v>19.99</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="5">
-        <v>45558.0</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="6">
-        <v>59.99</v>
-      </c>
-      <c r="I6" s="6">
-        <v>59.99</v>
-      </c>
-      <c r="J6" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L6" s="9">
-        <f t="shared" si="2"/>
-        <v>59.99</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>1062.0</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="12">
-        <v>1057.0</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>21</v>
@@ -1085,42 +1105,42 @@
       <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="I7" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="L7" s="16">
-        <f t="shared" si="2"/>
-        <v>19.99</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="12" t="s">
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6">
+        <v>79.99</v>
+      </c>
+      <c r="I7" s="6">
+        <v>79.99</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="2"/>
+        <v>79.99</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>1058.0</v>
+        <v>1063.0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>15</v>
@@ -1143,7 +1163,7 @@
       <c r="I8" s="6">
         <v>79.99</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1155,24 +1175,24 @@
         <v>79.99</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>1059.0</v>
+        <v>1064.0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>16</v>
@@ -1184,12 +1204,12 @@
         <v>17</v>
       </c>
       <c r="H9" s="6">
-        <v>79.99</v>
+        <v>19.99</v>
       </c>
       <c r="I9" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="J9" s="11">
+        <v>19.99</v>
+      </c>
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1198,102 +1218,102 @@
       </c>
       <c r="L9" s="9">
         <f t="shared" si="2"/>
-        <v>79.99</v>
+        <v>19.99</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>1065.0</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="12">
-        <v>1060.0</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="I10" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="J10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="L10" s="16">
-        <f t="shared" si="2"/>
-        <v>19.99</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="6">
+        <v>79.99</v>
+      </c>
+      <c r="I10" s="6">
+        <v>79.99</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" si="2"/>
+        <v>79.99</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>1061.0</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="10" t="s">
+        <v>1066.0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45636.0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="I11" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="J11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L11" s="9">
-        <f t="shared" si="2"/>
-        <v>79.99</v>
-      </c>
       <c r="M11" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>23</v>
@@ -1301,13 +1321,13 @@
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <v>1062.0</v>
+        <v>1067.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5">
         <v>45636.0</v>
@@ -1322,12 +1342,12 @@
         <v>17</v>
       </c>
       <c r="H12" s="6">
-        <v>15.0</v>
+        <v>14.99</v>
       </c>
       <c r="I12" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="J12" s="11">
+        <v>14.99</v>
+      </c>
+      <c r="J12" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1336,10 +1356,10 @@
       </c>
       <c r="L12" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14.99</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>23</v>
@@ -1347,16 +1367,16 @@
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <v>1063.0</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>48</v>
+        <v>1068.0</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D13" s="5">
-        <v>45636.0</v>
+        <v>45594.0</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
@@ -1368,24 +1388,24 @@
         <v>17</v>
       </c>
       <c r="H13" s="6">
-        <v>14.99</v>
+        <v>59.99</v>
       </c>
       <c r="I13" s="6">
-        <v>14.99</v>
-      </c>
-      <c r="J13" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40.19</v>
+      </c>
+      <c r="J13" s="13">
+        <f t="shared" si="1"/>
+        <v>19.8</v>
       </c>
       <c r="K13" s="8">
         <v>1.0</v>
       </c>
       <c r="L13" s="9">
         <f t="shared" si="2"/>
-        <v>14.99</v>
+        <v>40.19</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>23</v>
@@ -1393,64 +1413,64 @@
     </row>
     <row r="14">
       <c r="A14" s="4">
-        <v>1064.0</v>
+        <v>1069.0</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45562.0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="I14" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" si="2"/>
+        <v>49.99</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5">
-        <v>45594.0</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="6">
-        <v>59.99</v>
-      </c>
-      <c r="I14" s="6">
-        <v>41.99</v>
-      </c>
-      <c r="J14" s="7">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="K14" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L14" s="9">
-        <f t="shared" si="2"/>
-        <v>41.99</v>
-      </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4">
-        <v>1065.0</v>
-      </c>
-      <c r="B15" s="4" t="s">
+        <v>1070.0</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="5">
-        <v>45562.0</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1460,84 +1480,84 @@
         <v>17</v>
       </c>
       <c r="H15" s="6">
-        <v>49.99</v>
+        <v>79.99</v>
       </c>
       <c r="I15" s="6">
-        <v>29.99</v>
+        <v>79.99</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K15" s="8">
         <v>1.0</v>
       </c>
       <c r="L15" s="9">
         <f t="shared" si="2"/>
-        <v>29.99</v>
+        <v>79.99</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>53</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4">
-        <v>1066.0</v>
-      </c>
-      <c r="B16" s="10" t="s">
+        <v>1071.0</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5">
+        <v>36637.0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="6">
+        <v>9.99</v>
+      </c>
+      <c r="I16" s="6">
+        <v>9.99</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L16" s="9">
+        <f t="shared" si="2"/>
+        <v>9.99</v>
+      </c>
+      <c r="M16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="I16" s="6">
-        <v>79.99</v>
-      </c>
-      <c r="J16" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L16" s="9">
-        <f t="shared" si="2"/>
-        <v>79.99</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>23</v>
+      <c r="N16" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4">
-        <v>1067.0</v>
+        <v>1072.0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5">
         <v>45611.0</v>
@@ -1555,35 +1575,35 @@
         <v>17.99</v>
       </c>
       <c r="I17" s="6">
-        <v>15.29</v>
+        <v>17.99</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="1"/>
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="K17" s="8">
         <v>1.0</v>
       </c>
       <c r="L17" s="9">
         <f t="shared" si="2"/>
-        <v>15.29</v>
-      </c>
-      <c r="M17" s="17" t="s">
+        <v>17.99</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="N17" s="17" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="4">
+        <v>1073.0</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="12">
-        <v>1068.0</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="C18" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5">
         <v>45611.0</v>
@@ -1601,81 +1621,81 @@
         <v>19.99</v>
       </c>
       <c r="I18" s="6">
-        <v>16.99</v>
+        <v>19.99</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K18" s="8">
         <v>1.0</v>
       </c>
       <c r="L18" s="9">
         <f t="shared" si="2"/>
-        <v>16.99</v>
-      </c>
-      <c r="M18" s="17" t="s">
+        <v>19.99</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4">
-        <v>1069.0</v>
-      </c>
-      <c r="B19" s="12" t="s">
+        <v>1074.0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" s="5">
+        <v>39640.0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="6">
+        <v>9.99</v>
+      </c>
+      <c r="I19" s="6">
+        <v>9.99</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L19" s="9">
+        <f t="shared" si="2"/>
+        <v>9.99</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="18">
-        <v>39640.0</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="14">
-        <v>9.99</v>
-      </c>
-      <c r="I19" s="14">
-        <v>9.99</v>
-      </c>
-      <c r="J19" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="L19" s="16">
-        <f t="shared" si="2"/>
-        <v>9.99</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N19" s="12" t="s">
+      <c r="N19" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4">
-        <v>1070.0</v>
+        <v>1075.0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5">
         <v>45470.0</v>
@@ -1695,7 +1715,7 @@
       <c r="I20" s="6">
         <v>49.99</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1707,7 +1727,7 @@
         <v>49.99</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>30</v>
@@ -1715,10 +1735,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4">
-        <v>1071.0</v>
+        <v>1076.0</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>15</v>
@@ -1741,7 +1761,7 @@
       <c r="I21" s="6">
         <v>79.99</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1753,7 +1773,7 @@
         <v>79.99</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>23</v>
@@ -1761,71 +1781,71 @@
     </row>
     <row r="22">
       <c r="A22" s="4">
-        <v>1072.0</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="10" t="s">
+        <v>1077.0</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="17">
         <v>45687.0</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="E22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>17</v>
       </c>
       <c r="H22" s="6">
         <v>19.99</v>
       </c>
       <c r="I22" s="6">
-        <v>16.99</v>
+        <v>19.99</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K22" s="8">
         <v>1.0</v>
       </c>
       <c r="L22" s="9">
         <f t="shared" si="2"/>
-        <v>16.99</v>
+        <v>19.99</v>
       </c>
       <c r="M22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N22" s="4" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" s="18">
+        <v>1078.0</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4">
-        <v>1073.0</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>73</v>
+      <c r="C23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H23" s="6">
         <v>39.99</v>
@@ -1833,7 +1853,7 @@
       <c r="I23" s="6">
         <v>39.99</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1845,171 +1865,171 @@
         <v>39.99</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4">
-        <v>1074.0</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="18">
+        <v>1079.0</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="11">
+        <v>45720.0</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="6">
+        <v>29.99</v>
+      </c>
+      <c r="I24" s="6">
+        <v>29.99</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L24" s="9">
+        <f t="shared" si="2"/>
+        <v>29.99</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="18">
+        <v>1080.0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="6">
+        <v>19.99</v>
+      </c>
+      <c r="I25" s="6">
+        <v>19.99</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L25" s="9">
+        <f t="shared" si="2"/>
+        <v>19.99</v>
+      </c>
+      <c r="M25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="6">
-        <v>39.99</v>
-      </c>
-      <c r="I24" s="6">
-        <v>39.99</v>
-      </c>
-      <c r="J24" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L24" s="9">
-        <f t="shared" si="2"/>
-        <v>39.99</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4">
-        <v>1075.0</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="N25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="6">
-        <v>39.99</v>
-      </c>
-      <c r="I25" s="6">
-        <v>15.99</v>
-      </c>
-      <c r="J25" s="7">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="K25" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L25" s="9">
-        <f t="shared" si="2"/>
-        <v>15.99</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4">
-        <v>1076.0</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H26" s="6">
         <v>39.99</v>
       </c>
       <c r="I26" s="6">
-        <v>15.99</v>
+        <v>39.99</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K26" s="8">
         <v>1.0</v>
       </c>
       <c r="L26" s="9">
         <f t="shared" si="2"/>
-        <v>15.99</v>
+        <v>39.99</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4">
-        <v>1077.0</v>
+      <c r="A27" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>72</v>
-      </c>
       <c r="E27" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H27" s="6">
         <v>39.99</v>
@@ -2017,7 +2037,7 @@
       <c r="I27" s="6">
         <v>39.99</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2029,133 +2049,133 @@
         <v>39.99</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4">
-        <v>1078.0</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>79</v>
+      <c r="A28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H28" s="6">
         <v>39.99</v>
       </c>
       <c r="I28" s="6">
-        <v>29.99</v>
-      </c>
-      <c r="J28" s="7">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>19.99</v>
+      </c>
+      <c r="J28" s="13">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="K28" s="8">
         <v>1.0</v>
       </c>
       <c r="L28" s="9">
         <f t="shared" si="2"/>
-        <v>29.99</v>
+        <v>19.99</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4">
-        <v>1079.0</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>17</v>
+      <c r="A29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="H29" s="6">
         <v>39.99</v>
       </c>
       <c r="I29" s="6">
-        <v>39.99</v>
-      </c>
-      <c r="J29" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19.99</v>
+      </c>
+      <c r="J29" s="13">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="K29" s="8">
         <v>1.0</v>
       </c>
       <c r="L29" s="9">
         <f t="shared" si="2"/>
-        <v>39.99</v>
+        <v>19.99</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4">
-        <v>1080.0</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="13">
-        <v>45720.0</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>17</v>
+      <c r="A30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="H30" s="6">
-        <v>29.99</v>
+        <v>39.99</v>
       </c>
       <c r="I30" s="6">
-        <v>29.99</v>
-      </c>
-      <c r="J30" s="11">
+        <v>39.99</v>
+      </c>
+      <c r="J30" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2164,122 +2184,101 @@
       </c>
       <c r="L30" s="9">
         <f t="shared" si="2"/>
-        <v>29.99</v>
+        <v>39.99</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="12">
-        <v>1081.0</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="5">
-        <v>38296.0</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>17</v>
+      <c r="D31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="H31" s="6">
-        <v>26.99</v>
+        <v>39.99</v>
       </c>
       <c r="I31" s="6">
-        <v>26.99</v>
-      </c>
-      <c r="J31" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.99</v>
+      </c>
+      <c r="J31" s="13">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="K31" s="8">
         <v>1.0</v>
       </c>
       <c r="L31" s="9">
         <f t="shared" si="2"/>
-        <v>26.99</v>
+        <v>29.99</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="12">
-        <v>1082.0</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="I32" s="14">
-        <v>19.99</v>
-      </c>
-      <c r="J32" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="L32" s="16">
-        <f t="shared" si="2"/>
-        <v>19.99</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="23">
+        <f t="shared" ref="H32:I32" si="3">SUM(H2:H31)</f>
+        <v>1277.71</v>
+      </c>
+      <c r="I32" s="23">
+        <f t="shared" si="3"/>
+        <v>1167.91</v>
+      </c>
+      <c r="J32" s="23">
+        <f t="shared" si="1"/>
+        <v>109.8</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
     </row>
     <row r="33">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
@@ -2327,203 +2326,209 @@
     </row>
     <row r="35">
       <c r="A35" s="24">
-        <v>1051.0</v>
-      </c>
-      <c r="B35" s="24" t="s">
+        <v>1054.0</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="26">
+        <v>40501.0</v>
+      </c>
+      <c r="E35" s="26">
+        <v>45664.0</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="27">
+        <v>39.99</v>
+      </c>
+      <c r="I35" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="J35" s="27">
+        <f>H35-I35</f>
+        <v>39.99</v>
+      </c>
+      <c r="K35" s="28">
+        <v>1.0</v>
+      </c>
+      <c r="L35" s="27">
+        <f t="shared" ref="L35:L37" si="4">I35/K35</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="N35" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4">
+        <v>1055.0</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="5">
+        <v>45129.0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>45692.0</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="6">
+        <v>39.99</v>
+      </c>
+      <c r="I36" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="J36" s="6">
+        <v>39.99</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="L36" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="25">
-        <v>45716.0</v>
-      </c>
-      <c r="E35" s="25">
-        <v>45716.0</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="26">
-        <v>59.99</v>
-      </c>
-      <c r="I35" s="26">
+      <c r="N36" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4">
+        <v>1056.0</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="5">
+        <v>44798.0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>45692.0</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="6">
+        <v>39.99</v>
+      </c>
+      <c r="I37" s="6">
         <v>0.0</v>
       </c>
-      <c r="J35" s="26">
-        <f>H35-I35</f>
-        <v>59.99</v>
-      </c>
-      <c r="K35" s="27">
-        <v>1.0</v>
-      </c>
-      <c r="L35" s="28">
-        <f>I35/K35</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="N35" s="24" t="s">
+      <c r="J37" s="6">
+        <v>39.99</v>
+      </c>
+      <c r="K37" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="L37" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N37" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="21"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="30" t="s">
+    <row r="38">
+      <c r="A38" s="4"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C39" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D39" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E39" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F39" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G39" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H39" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="31" t="s">
+      <c r="I39" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="30" t="s">
+      <c r="J39" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="K37" s="30" t="s">
+      <c r="K39" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L37" s="32" t="s">
+      <c r="L39" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="30" t="s">
+      <c r="M39" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N37" s="30" t="s">
+      <c r="N39" s="30" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="22"/>
-      <c r="B38" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="6">
-        <v>59.99</v>
-      </c>
-      <c r="I38" s="6">
-        <v>59.99</v>
-      </c>
-      <c r="J38" s="9">
-        <f t="shared" ref="J38:J42" si="3">H38-I38</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L38" s="9">
-        <f t="shared" ref="L38:L42" si="4">I38/K38</f>
-        <v>59.99</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="22"/>
-      <c r="B39" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="6">
-        <v>34.99</v>
-      </c>
-      <c r="I39" s="6">
-        <v>34.99</v>
-      </c>
-      <c r="J39" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K39" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L39" s="9">
-        <f t="shared" si="4"/>
-        <v>34.99</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="33"/>
+        <v>93</v>
+      </c>
+      <c r="D40" s="21"/>
       <c r="E40" s="4" t="s">
         <v>16</v>
       </c>
@@ -2534,24 +2539,24 @@
         <v>17</v>
       </c>
       <c r="H40" s="6">
-        <v>49.99</v>
+        <v>59.99</v>
       </c>
       <c r="I40" s="6">
-        <v>49.99</v>
+        <v>59.99</v>
       </c>
       <c r="J40" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J40:J44" si="5">H40-I40</f>
         <v>0</v>
       </c>
       <c r="K40" s="8">
         <v>1.0</v>
       </c>
       <c r="L40" s="9">
-        <f t="shared" si="4"/>
-        <v>49.99</v>
+        <f t="shared" ref="L40:L44" si="6">I40/K40</f>
+        <v>59.99</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>30</v>
@@ -2560,10 +2565,10 @@
     <row r="41">
       <c r="A41" s="22"/>
       <c r="B41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D41" s="33"/>
       <c r="E41" s="4" t="s">
@@ -2576,24 +2581,24 @@
         <v>17</v>
       </c>
       <c r="H41" s="6">
-        <v>49.99</v>
+        <v>34.99</v>
       </c>
       <c r="I41" s="6">
-        <v>49.99</v>
+        <v>34.99</v>
       </c>
       <c r="J41" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K41" s="8">
         <v>1.0</v>
       </c>
       <c r="L41" s="9">
-        <f t="shared" si="4"/>
-        <v>49.99</v>
+        <f t="shared" si="6"/>
+        <v>34.99</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>30</v>
@@ -2602,42 +2607,126 @@
     <row r="42">
       <c r="A42" s="22"/>
       <c r="B42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="33"/>
+      <c r="E42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="I42" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="J42" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L42" s="9">
+        <f t="shared" si="6"/>
+        <v>49.99</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="22"/>
+      <c r="B43" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H42" s="6">
+      <c r="C43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="I43" s="6">
+        <v>49.99</v>
+      </c>
+      <c r="J43" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L43" s="9">
+        <f t="shared" si="6"/>
+        <v>49.99</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="22"/>
+      <c r="B44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="6">
         <v>54.99</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I44" s="6">
         <v>54.99</v>
       </c>
-      <c r="J42" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K42" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="L42" s="9">
-        <f t="shared" si="4"/>
+      <c r="J44" s="9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="L44" s="9">
+        <f t="shared" si="6"/>
         <v>54.99</v>
       </c>
-      <c r="M42" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N42" s="4" t="s">
+      <c r="M44" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N44" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>